<commit_message>
submit all the new results
new results
</commit_message>
<xml_diff>
--- a/09_IMA/MORGAN/Results/results_RQ3/CAEX/results_RQ3.xlsx
+++ b/09_IMA/MORGAN/Results/results_RQ3/CAEX/results_RQ3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vitto\Desktop\github\modelingOperationRec_IST\09_IMA\MORGAN\Results\results_RQ3\CAEX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C760F0B7-AB08-4BDA-B170-359E6E44B61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3ADAF3B-73ED-432E-9C52-E4EA92E3F356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -399,13 +399,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.7037037037037002</c:v>
+                  <c:v>29.629629629629601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222201</c:v>
+                  <c:v>61.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7777777777777701</c:v>
+                  <c:v>39.072039072038997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1773,13 +1773,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>3.7037037037037002</c:v>
+                  <c:v>29.629629629629601</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2222222222222201</c:v>
+                  <c:v>61.1111111111111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.7777777777777701</c:v>
+                  <c:v>39.072039072038997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5423,8 +5423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5560,19 +5560,19 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>3.7037037037037002</v>
+        <v>29.629629629629601</v>
       </c>
       <c r="D6">
-        <v>2.2222222222222201</v>
+        <v>61.1111111111111</v>
       </c>
       <c r="E6">
-        <v>2.7777777777777701</v>
+        <v>39.072039072038997</v>
       </c>
       <c r="F6">
-        <v>4.5781850814819301E-2</v>
+        <v>4.7577540079752602E-2</v>
       </c>
       <c r="G6">
-        <v>3.8493080933888701</v>
+        <v>4.2496791680653798</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">
@@ -5705,8 +5705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3ADEAC9-6465-4B92-99E1-48C53161746C}">
   <dimension ref="A1:P20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="C2:G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5842,19 +5842,19 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>3.7037037037037002</v>
+        <v>29.629629629629601</v>
       </c>
       <c r="D6">
-        <v>2.2222222222222201</v>
+        <v>61.1111111111111</v>
       </c>
       <c r="E6">
-        <v>2.7777777777777701</v>
+        <v>39.072039072038997</v>
       </c>
       <c r="F6">
-        <v>4.5781850814819301E-2</v>
+        <v>4.7577540079752602E-2</v>
       </c>
       <c r="G6">
-        <v>3.8493080933888701</v>
+        <v>4.2496791680653798</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.3">

</xml_diff>